<commit_message>
rename cytof_s1609 -> cytof_s1609_gd2car
</commit_message>
<xml_diff>
--- a/template_examples/cytof_s1609_gd2car_template.xlsx
+++ b/template_examples/cytof_s1609_gd2car_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/VSCodeProjects/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD12E25-1588-1641-AC22-770CC291D92C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E8B16E-18DD-7D40-886D-77599031DC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="3920" windowWidth="22160" windowHeight="12380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1040" yWindow="3920" windowWidth="22160" windowHeight="12380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
@@ -112,16 +112,48 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Path to a file on a user's computer.
-In .fcs format</t>
+          <t xml:space="preserve">Path to a file on a user's computer.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>In .fcs format</t>
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{48A26E9E-1E11-3C4B-8B3D-1A4836A5A9B2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Path to a file on a user's computer.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>In .fcs format</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -134,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -147,7 +179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -160,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -173,7 +205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -186,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -199,7 +231,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -212,7 +244,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -225,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -240,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -263,7 +295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="E19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -277,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -290,7 +322,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -303,7 +335,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
+    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -316,7 +348,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -461,7 +493,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4217" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4220" uniqueCount="128">
   <si>
     <t>LEGEND</t>
   </si>
@@ -840,6 +872,12 @@
   </si>
   <si>
     <t>146Nb</t>
+  </si>
+  <si>
+    <t>Controls spike-in fcs filename(s)</t>
+  </si>
+  <si>
+    <t>control1-vericell.fcs,control2-vericell.fcs</t>
   </si>
 </sst>
 </file>
@@ -1340,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2018"/>
+  <dimension ref="A1:I2019"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1437,15 +1475,15 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>88</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>126</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1453,10 +1491,10 @@
         <v>88</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="6">
-        <v>43355</v>
+        <v>18</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1464,10 +1502,10 @@
         <v>88</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>101</v>
+        <v>20</v>
+      </c>
+      <c r="C11" s="6">
+        <v>43355</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1475,10 +1513,10 @@
         <v>88</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="2" t="b">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1486,10 +1524,10 @@
         <v>88</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>79</v>
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1497,7 +1535,7 @@
         <v>88</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>79</v>
@@ -1508,102 +1546,84 @@
         <v>88</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="I19" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" s="7" t="s">
+    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C20" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D20" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>107</v>
-      </c>
-      <c r="F19" t="s">
-        <v>108</v>
-      </c>
-      <c r="G19" t="s">
-        <v>101</v>
-      </c>
-      <c r="H19" t="s">
-        <v>109</v>
-      </c>
-      <c r="I19" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E20" t="s">
-        <v>111</v>
       </c>
       <c r="F20" t="s">
         <v>108</v>
@@ -1615,13 +1635,37 @@
         <v>109</v>
       </c>
       <c r="I20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>93</v>
       </c>
+      <c r="B21" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" t="s">
+        <v>111</v>
+      </c>
+      <c r="F21" t="s">
+        <v>108</v>
+      </c>
+      <c r="G21" t="s">
+        <v>101</v>
+      </c>
+      <c r="H21" t="s">
+        <v>109</v>
+      </c>
+      <c r="I21" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -11605,17 +11649,22 @@
     </row>
     <row r="2018" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2018" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2019" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2019" t="s">
         <v>93</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:I18"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{AAE1337E-7421-AF46-8151-22B72A38EB45}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{AAE1337E-7421-AF46-8151-22B72A38EB45}">
       <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>
@@ -11628,7 +11677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:J4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
remove 'intermediate fcs' optional field
</commit_message>
<xml_diff>
--- a/template_examples/cytof_s1609_gd2car_template.xlsx
+++ b/template_examples/cytof_s1609_gd2car_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/VSCodeProjects/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E8B16E-18DD-7D40-886D-77599031DC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2955B33-F3C3-9142-92D0-DC83FA832F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="3920" windowWidth="22160" windowHeight="12380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -257,22 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Path to a file on a User's computer. 
-This .fcs file is an intermediate file that has been normalized, concatenated, and debarcoded, but has the veri-cells and has not been cleaned up.
-In .fcs format</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -295,7 +280,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -309,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="E19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -322,7 +307,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -335,7 +320,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
+    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -348,7 +333,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -493,7 +478,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4220" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4217" uniqueCount="126">
   <si>
     <t>LEGEND</t>
   </si>
@@ -808,13 +793,7 @@
     <t>CTTTPP111.00</t>
   </si>
   <si>
-    <t>sample1_n.fcs</t>
-  </si>
-  <si>
     <t>CTTTPP121.00</t>
-  </si>
-  <si>
-    <t>sample2_n.fcs</t>
   </si>
   <si>
     <t>sample1.fcs</t>
@@ -1013,7 +992,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1037,6 +1016,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1378,18 +1360,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2019"/>
+  <dimension ref="A1:H2019"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="101" width="30.6640625" customWidth="1"/>
+    <col min="1" max="100" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>86</v>
       </c>
@@ -1472,7 +1454,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="33" thickBot="1" x14ac:dyDescent="0.25">
@@ -1480,10 +1462,10 @@
         <v>88</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1563,24 +1545,23 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>89</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9" t="s">
+      <c r="C18" s="10"/>
+      <c r="D18" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>92</v>
       </c>
@@ -1588,28 +1569,25 @@
         <v>35</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I19" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>93</v>
       </c>
@@ -1617,107 +1595,101 @@
         <v>103</v>
       </c>
       <c r="C20" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" t="s">
+        <v>101</v>
+      </c>
+      <c r="G20" t="s">
+        <v>107</v>
+      </c>
+      <c r="H20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="C21" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21" t="s">
         <v>107</v>
       </c>
-      <c r="F20" t="s">
-        <v>108</v>
-      </c>
-      <c r="G20" t="s">
-        <v>101</v>
-      </c>
-      <c r="H20" t="s">
-        <v>109</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="H21" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" t="s">
-        <v>111</v>
-      </c>
-      <c r="F21" t="s">
-        <v>108</v>
-      </c>
-      <c r="G21" t="s">
-        <v>101</v>
-      </c>
-      <c r="H21" t="s">
-        <v>109</v>
-      </c>
-      <c r="I21" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>93</v>
       </c>
@@ -11658,10 +11630,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:I18"/>
+  <mergeCells count="2">
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:H18"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{AAE1337E-7421-AF46-8151-22B72A38EB45}">
@@ -11690,17 +11661,17 @@
       <c r="A1" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -11739,25 +11710,25 @@
         <v>93</v>
       </c>
       <c r="B3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" t="s">
         <v>116</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>117</v>
-      </c>
-      <c r="D3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E3" t="s">
-        <v>119</v>
       </c>
       <c r="F3">
         <v>3983272</v>
       </c>
       <c r="G3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I3" t="s">
         <v>81</v>
@@ -11771,25 +11742,25 @@
         <v>93</v>
       </c>
       <c r="B4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" t="s">
         <v>122</v>
-      </c>
-      <c r="C4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" t="s">
-        <v>124</v>
       </c>
       <c r="F4">
         <v>1231272</v>
       </c>
       <c r="G4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I4" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
add target reuse test
</commit_message>
<xml_diff>
--- a/template_examples/cytof_s1609_gd2car_template.xlsx
+++ b/template_examples/cytof_s1609_gd2car_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/VSCodeProjects/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2955B33-F3C3-9142-92D0-DC83FA832F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E78BBC-065E-854F-BC66-409830E63FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="3920" windowWidth="22160" windowHeight="12380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7640" yWindow="3640" windowWidth="22160" windowHeight="12380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
@@ -478,7 +478,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4217" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4225" uniqueCount="130">
   <si>
     <t>LEGEND</t>
   </si>
@@ -835,9 +835,6 @@
     <t>C8-ABC</t>
   </si>
   <si>
-    <t>146Nd</t>
-  </si>
-  <si>
     <t>100X</t>
   </si>
   <si>
@@ -850,20 +847,35 @@
     <t>C8-AB123</t>
   </si>
   <si>
-    <t>146Nb</t>
-  </si>
-  <si>
     <t>Controls spike-in fcs filename(s)</t>
   </si>
   <si>
     <t>control1-vericell.fcs,control2-vericell.fcs</t>
+  </si>
+  <si>
+    <t>3146001B</t>
+  </si>
+  <si>
+    <t>0.2 uL</t>
+  </si>
+  <si>
+    <t>113In</t>
+  </si>
+  <si>
+    <t>115In</t>
+  </si>
+  <si>
+    <t>141Pr</t>
+  </si>
+  <si>
+    <t>Barcoding</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -905,6 +917,12 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -992,7 +1010,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1021,6 +1039,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1462,10 +1487,10 @@
         <v>88</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -11648,8 +11673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2002"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11724,11 +11749,11 @@
       <c r="F3">
         <v>3983272</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" t="s">
         <v>118</v>
-      </c>
-      <c r="H3" t="s">
-        <v>119</v>
       </c>
       <c r="I3" t="s">
         <v>81</v>
@@ -11742,25 +11767,25 @@
         <v>93</v>
       </c>
       <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" t="s">
         <v>120</v>
-      </c>
-      <c r="C4" t="s">
-        <v>121</v>
       </c>
       <c r="D4" t="s">
         <v>116</v>
       </c>
       <c r="E4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F4">
         <v>1231272</v>
       </c>
-      <c r="G4" t="s">
-        <v>123</v>
+      <c r="G4" s="11" t="s">
+        <v>127</v>
       </c>
       <c r="H4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I4" t="s">
         <v>81</v>
@@ -11772,6 +11797,33 @@
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>93</v>
+      </c>
+      <c r="B5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F5" s="13">
+        <v>1671716</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="H5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -21772,13 +21824,13 @@
           <x14:formula1>
             <xm:f>'Data Dictionary'!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>I5:I2002</xm:sqref>
+          <xm:sqref>I6:I2002</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>'Data Dictionary'!$E$2:$E$4</xm:f>
           </x14:formula1>
-          <xm:sqref>J5:J2002</xm:sqref>
+          <xm:sqref>J6:J2002</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>